<commit_message>
2017 is done -> 2014 LOAD IN THE LOGGING STATUS ECT
</commit_message>
<xml_diff>
--- a/Kelly_errors_to_fix.xlsx
+++ b/Kelly_errors_to_fix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10911"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelly\Documents\Belize-MP-Bruno-Boos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elise/Desktop/MP/Belize-MP-Bruno-Boos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3020643-3A54-40D5-9F42-4A4A33ABE219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D143D99-C3FA-7E42-AF40-723F70D328C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11470" yWindow="100" windowWidth="7720" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11480" yWindow="500" windowWidth="15740" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="50">
   <si>
     <t>Year</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>I think the year is supposed to be 2017</t>
+  </si>
+  <si>
+    <t>This is pic 10100232</t>
   </si>
 </sst>
 </file>
@@ -545,22 +548,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:M128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="76" workbookViewId="0">
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,7 +592,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -603,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -620,7 +623,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -637,7 +640,7 @@
         <v>42221</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -654,7 +657,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2016</v>
       </c>
@@ -680,7 +683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>2016</v>
       </c>
@@ -706,7 +709,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2016</v>
       </c>
@@ -732,7 +735,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2016</v>
       </c>
@@ -758,7 +761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>2016</v>
       </c>
@@ -781,7 +784,7 @@
         <v>42472</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>2016</v>
       </c>
@@ -807,7 +810,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>2016</v>
       </c>
@@ -833,7 +836,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2016</v>
       </c>
@@ -859,7 +862,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2016</v>
       </c>
@@ -882,7 +885,7 @@
         <v>40915</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2016</v>
       </c>
@@ -905,7 +908,7 @@
         <v>40914</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>2017</v>
       </c>
@@ -928,7 +931,7 @@
         <v>43043</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>2017</v>
       </c>
@@ -951,7 +954,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>2017</v>
       </c>
@@ -974,7 +977,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>2017</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>2017</v>
       </c>
@@ -1020,7 +1023,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>2017</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>42954</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>2017</v>
       </c>
@@ -1060,7 +1063,7 @@
         <v>42956</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>2017</v>
       </c>
@@ -1080,7 +1083,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>2017</v>
       </c>
@@ -1100,7 +1103,7 @@
         <v>42951</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>2017</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>42957</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>2017</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>43015</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>2017</v>
       </c>
@@ -1160,7 +1163,7 @@
         <v>43017</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>2017</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>43013</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>2017</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>2017</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>43029</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>2017</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>43036</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>2017</v>
       </c>
@@ -1260,7 +1263,7 @@
         <v>43037</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>2017</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>43019</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>2017</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>2017</v>
       </c>
@@ -1320,7 +1323,7 @@
         <v>43019</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>2017</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>2017</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>2017</v>
       </c>
@@ -1380,7 +1383,7 @@
         <v>43018</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>2017</v>
       </c>
@@ -1400,7 +1403,7 @@
         <v>43014</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>2017</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>2017</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>43032</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>2017</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>43034</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>2017</v>
       </c>
@@ -1480,7 +1483,7 @@
         <v>43014</v>
       </c>
     </row>
-    <row r="44" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>2017</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>2017</v>
       </c>
@@ -1520,7 +1523,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>2017</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>43022</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>2017</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>43035</v>
       </c>
     </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>2017</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>43035</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>2017</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>2017</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>43012</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>2017</v>
       </c>
@@ -1640,7 +1643,7 @@
         <v>43016</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>2017</v>
       </c>
@@ -1660,7 +1663,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>2017</v>
       </c>
@@ -1680,7 +1683,7 @@
         <v>43030</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>2017</v>
       </c>
@@ -1700,7 +1703,7 @@
         <v>43035</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>2017</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>43039</v>
       </c>
     </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>2017</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>2017</v>
       </c>
@@ -1760,7 +1763,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>2017</v>
       </c>
@@ -1780,7 +1783,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>2017</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>2017</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>43029</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>2017</v>
       </c>
@@ -1840,7 +1843,7 @@
         <v>43033</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>2017</v>
       </c>
@@ -1860,7 +1863,7 @@
         <v>43033</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>2017</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>43037</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>2017</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>43030</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>2017</v>
       </c>
@@ -1920,7 +1923,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>2017</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>43019</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>2017</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>2017</v>
       </c>
@@ -1985,8 +1988,11 @@
       <c r="I68" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M68" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>2017</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>2017</v>
       </c>
@@ -2029,7 +2035,7 @@
         <v>43005</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>2017</v>
       </c>
@@ -2049,7 +2055,7 @@
         <v>43027</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>2017</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>43010</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>2017</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>2017</v>
       </c>
@@ -2109,7 +2115,7 @@
         <v>43010</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>2017</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>43001</v>
       </c>
     </row>
-    <row r="76" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>2017</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>43002</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>2017</v>
       </c>
@@ -2169,7 +2175,7 @@
         <v>43002</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>2017</v>
       </c>
@@ -2189,7 +2195,7 @@
         <v>43003</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>2017</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>43006</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>2017</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>43006</v>
       </c>
     </row>
-    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>2017</v>
       </c>
@@ -2249,7 +2255,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>2017</v>
       </c>
@@ -2269,7 +2275,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>2017</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>2017</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>43021</v>
       </c>
     </row>
-    <row r="85" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <v>2017</v>
       </c>
@@ -2329,7 +2335,7 @@
         <v>43022</v>
       </c>
     </row>
-    <row r="86" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>2017</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>2017</v>
       </c>
@@ -2369,7 +2375,7 @@
         <v>43025</v>
       </c>
     </row>
-    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>2017</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>43025</v>
       </c>
     </row>
-    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>2017</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>43028</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>2017</v>
       </c>
@@ -2429,7 +2435,7 @@
         <v>43028</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>2017</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>43003</v>
       </c>
     </row>
-    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>2017</v>
       </c>
@@ -2469,7 +2475,7 @@
         <v>43014</v>
       </c>
     </row>
-    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <v>2017</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>43026</v>
       </c>
     </row>
-    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>2017</v>
       </c>
@@ -2509,7 +2515,7 @@
         <v>42923</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>2017</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>42915</v>
       </c>
     </row>
-    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>2017</v>
       </c>
@@ -2549,7 +2555,7 @@
         <v>42917</v>
       </c>
     </row>
-    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>2017</v>
       </c>
@@ -2569,7 +2575,7 @@
         <v>42919</v>
       </c>
     </row>
-    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <v>2017</v>
       </c>
@@ -2589,7 +2595,7 @@
         <v>42923</v>
       </c>
     </row>
-    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <v>2017</v>
       </c>
@@ -2609,7 +2615,7 @@
         <v>42922</v>
       </c>
     </row>
-    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>2017</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>42917</v>
       </c>
     </row>
-    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <v>2017</v>
       </c>
@@ -2649,7 +2655,7 @@
         <v>42922</v>
       </c>
     </row>
-    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
         <v>2017</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>42922</v>
       </c>
     </row>
-    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <v>2017</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>43030</v>
       </c>
     </row>
-    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <v>2017</v>
       </c>
@@ -2709,7 +2715,7 @@
         <v>43034</v>
       </c>
     </row>
-    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="5">
         <v>2017</v>
       </c>
@@ -2729,7 +2735,7 @@
         <v>43016</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106" s="5">
         <v>2017</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>43037</v>
       </c>
     </row>
-    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>2017</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="108" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>2017</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>43026</v>
       </c>
     </row>
-    <row r="109" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>2017</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>43020</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <v>2017</v>
       </c>
@@ -2829,7 +2835,7 @@
         <v>43028</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <v>2017</v>
       </c>
@@ -2849,7 +2855,7 @@
         <v>43030</v>
       </c>
     </row>
-    <row r="112" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5">
         <v>2017</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>43024</v>
       </c>
     </row>
-    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <v>2017</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>42995</v>
       </c>
     </row>
-    <row r="114" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>2017</v>
       </c>
@@ -2909,7 +2915,7 @@
         <v>42998</v>
       </c>
     </row>
-    <row r="115" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <v>2017</v>
       </c>
@@ -2929,7 +2935,7 @@
         <v>43018</v>
       </c>
     </row>
-    <row r="116" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5">
         <v>2017</v>
       </c>
@@ -2949,7 +2955,7 @@
         <v>42982</v>
       </c>
     </row>
-    <row r="117" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>2017</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>43006</v>
       </c>
     </row>
-    <row r="118" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5">
         <v>2017</v>
       </c>
@@ -2989,7 +2995,7 @@
         <v>43016</v>
       </c>
     </row>
-    <row r="119" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <v>2017</v>
       </c>
@@ -3009,7 +3015,7 @@
         <v>42982</v>
       </c>
     </row>
-    <row r="120" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <v>2017</v>
       </c>
@@ -3029,7 +3035,7 @@
         <v>42992</v>
       </c>
     </row>
-    <row r="121" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <v>2017</v>
       </c>
@@ -3049,7 +3055,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <v>2017</v>
       </c>
@@ -3069,7 +3075,7 @@
         <v>43000</v>
       </c>
     </row>
-    <row r="123" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <v>2017</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>43019</v>
       </c>
     </row>
-    <row r="124" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <v>2017</v>
       </c>
@@ -3109,7 +3115,7 @@
         <v>42996</v>
       </c>
     </row>
-    <row r="125" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <v>2017</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>43002</v>
       </c>
     </row>
-    <row r="126" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>2017</v>
       </c>
@@ -3149,7 +3155,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="127" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <v>2017</v>
       </c>
@@ -3169,7 +3175,7 @@
         <v>42982</v>
       </c>
     </row>
-    <row r="128" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <v>2017</v>
       </c>

</xml_diff>